<commit_message>
20190424 detp table semi project update
</commit_message>
<xml_diff>
--- a/dept_plan_table.xlsx
+++ b/dept_plan_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesson6_mac/git_work/study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C498A9E-48A9-364A-806D-88574E28DF27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39F2C24-4448-9E4D-A206-92C288BF8C66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="540" windowWidth="28300" windowHeight="16760" xr2:uid="{FF60E1AC-040A-EF43-8365-A6042912140D}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="16760" xr2:uid="{FF60E1AC-040A-EF43-8365-A6042912140D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>라이브러리</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -91,10 +91,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>bean</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>configuration</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -127,10 +123,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>xml 빈으로 설정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>sql 문 실행을 위해 필요한 인풋데이터 및 아웃풋데이터 설정</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -187,15 +179,30 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>bean.xml</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>mapper.xml</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>configuration.xml</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>template</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>중앙 허브 역할을 위한 설정 및 전역 설정 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구현체 설정 및 프로퍼티 설정</t>
+  </si>
+  <si>
+    <t>구현체 설정 및 프로퍼티 설정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DBtemplate.xml</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -324,7 +331,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -334,29 +341,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05010809-E4C4-A34C-878F-E6BF52176FE2}">
-  <dimension ref="B4:D35"/>
+  <dimension ref="B4:G35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -688,10 +701,10 @@
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="1" t="s">
@@ -731,17 +744,17 @@
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="6"/>
     </row>
@@ -750,7 +763,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="6"/>
     </row>
@@ -759,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="6"/>
     </row>
@@ -768,7 +781,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="6"/>
     </row>
@@ -777,187 +790,194 @@
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:7">
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="1" t="s">
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D21" s="6"/>
-    </row>
-    <row r="24" spans="2:4">
+      <c r="G21" s="12"/>
+    </row>
+    <row r="24" spans="2:7">
       <c r="B24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:7">
       <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
       <c r="B29" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
       <c r="B30" s="8"/>
       <c r="C30" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
       <c r="B31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
+        <v>36</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
       <c r="B32" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
@@ -968,12 +988,6 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>